<commit_message>
switched completely to xlsx i/o
</commit_message>
<xml_diff>
--- a/example/schedule.xlsx
+++ b/example/schedule.xlsx
@@ -9,12 +9,13 @@
     <sheet name="2019-02" r:id="rId3" sheetId="1"/>
     <sheet name="doctors.stats" r:id="rId4" sheetId="2"/>
     <sheet name="opt_parms" r:id="rId5" sheetId="3"/>
+    <sheet name="warnings" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="170">
   <si>
     <t>01</t>
   </si>
@@ -127,15 +128,18 @@
     <t>Cottle</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>U</t>
   </si>
   <si>
@@ -148,13 +152,13 @@
     <t>7</t>
   </si>
   <si>
-    <t>6</t>
+    <t>N2</t>
   </si>
   <si>
     <t>N1</t>
   </si>
   <si>
-    <t>N2</t>
+    <t>8</t>
   </si>
   <si>
     <t>4_2</t>
@@ -175,9 +179,6 @@
     <t>2019-02</t>
   </si>
   <si>
-    <t>role</t>
-  </si>
-  <si>
     <t>ward</t>
   </si>
   <si>
@@ -199,7 +200,7 @@
     <t>long_day_hours</t>
   </si>
   <si>
-    <t>fill_days_beyond_weekhours</t>
+    <t>fill_all_days</t>
   </si>
   <si>
     <t>shifts_carryover</t>
@@ -253,9 +254,6 @@
     <t>soft_requests_denied</t>
   </si>
   <si>
-    <t>AA</t>
-  </si>
-  <si>
     <t>TRUE</t>
   </si>
   <si>
@@ -296,6 +294,237 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>warnings</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>No more doctor found for 4, ward 4_2 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 7, ward 4_2 presence remains 1</t>
+  </si>
+  <si>
+    <t>No more doctor found for 6, ward 4_2 presence remains 1</t>
+  </si>
+  <si>
+    <t>No more doctor found for 8, ward 4_1 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 26, ward 4_1 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 11, ward 4_1 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 4, ward 12_2 presence remains 1</t>
+  </si>
+  <si>
+    <t>No more doctor found for 1, ward 12_2 presence remains 2</t>
+  </si>
+  <si>
+    <t>No more doctor found for 5, ward 12_2 presence remains 1</t>
+  </si>
+  <si>
+    <t>No more doctor found for 7, ward 12_2 presence remains 1</t>
+  </si>
+  <si>
+    <t>No more doctor found for 6, ward 12_2 presence remains 1</t>
+  </si>
+  <si>
+    <t>No more doctor found for 28, ward 12_2 presence remains 2</t>
+  </si>
+  <si>
+    <t>No more doctor found for 25, ward 12_2 presence remains 2</t>
+  </si>
+  <si>
+    <t>No more doctor found for 8, ward 12_2 presence remains 1</t>
+  </si>
+  <si>
+    <t>No more doctor found for 20, ward 12_2 presence remains 2</t>
+  </si>
+  <si>
+    <t>No more doctor found for 14, ward 4_3 presence remains 1</t>
+  </si>
+  <si>
+    <t>No more doctor found for 13, ward 4_3 presence remains 1</t>
+  </si>
+  <si>
+    <t>No more doctor found for 12, ward 4_3 presence remains 1</t>
+  </si>
+  <si>
+    <t>No more doctor found for 25, ward 4_3 presence remains 2</t>
+  </si>
+  <si>
+    <t>No more doctor found for 6, ward 4_3 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 8, ward 4_3 presence remains 2</t>
+  </si>
+  <si>
+    <t>No more doctor found for 22, ward 4_3 presence remains 1</t>
+  </si>
+  <si>
+    <t>No more doctor found for 7, ward 4_3 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 22, ward 6_3 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 18, ward 6_3 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 28, ward 6_3 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 25, ward 6_3 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 5, ward 6_3 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 14, ward 6_3 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 21, ward 6_3 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 26, ward 6_3 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 19, ward 6_3 presence remains 0</t>
+  </si>
+  <si>
+    <t>No more doctor found for 4, total presence remains 4</t>
+  </si>
+  <si>
+    <t>No more doctor found for 7, total presence remains 4</t>
+  </si>
+  <si>
+    <t>No more doctor found for 25, total presence remains 7</t>
+  </si>
+  <si>
+    <t>No more doctor found for 8, total presence remains 5</t>
+  </si>
+  <si>
+    <t>No more doctor found for 6, total presence remains 4</t>
+  </si>
+  <si>
+    <t>No more doctor found for 5, total presence remains 5</t>
+  </si>
+  <si>
+    <t>No more doctor found for 26, total presence remains 6</t>
+  </si>
+  <si>
+    <t>No more doctor found for 22, total presence remains 7</t>
+  </si>
+  <si>
+    <t>No more doctor found for 14, total presence remains 4</t>
+  </si>
+  <si>
+    <t>No more doctor found for 28, total presence remains 6</t>
+  </si>
+  <si>
+    <t>No more doctor found for 13, total presence remains 5</t>
+  </si>
+  <si>
+    <t>No more doctor found for 18, total presence remains 6</t>
+  </si>
+  <si>
+    <t>No more doctor found for 21, total presence remains 7</t>
+  </si>
+  <si>
+    <t>No more doctor found for 19, total presence remains 6</t>
+  </si>
+  <si>
+    <t>No more doctor found for 11, total presence remains 5</t>
+  </si>
+  <si>
+    <t>No more doctor found for 1, total presence remains 6</t>
+  </si>
+  <si>
+    <t>No more doctor found for 20, total presence remains 6</t>
+  </si>
+  <si>
+    <t>No more doctor found for 12, total presence remains 6</t>
   </si>
 </sst>
 </file>
@@ -611,7 +840,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.59375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="13.5" customWidth="true"/>
     <col min="2" max="2" width="4.5" customWidth="true"/>
     <col min="3" max="3" width="4.5" customWidth="true"/>
     <col min="4" max="4" width="4.5" customWidth="true"/>
@@ -642,9 +871,9 @@
     <col min="29" max="29" width="4.5" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.0" customHeight="true">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -731,7 +960,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15.0" customHeight="true">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -739,61 +968,61 @@
         <v>37</v>
       </c>
       <c r="C2" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="L2" t="s" s="6">
+        <v>46</v>
+      </c>
+      <c r="M2" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="O2" t="s" s="4">
         <v>42</v>
       </c>
-      <c r="D2" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s" s="4">
-        <v>40</v>
-      </c>
-      <c r="F2" t="s" s="4">
-        <v>40</v>
-      </c>
-      <c r="G2" t="s" s="4">
-        <v>40</v>
-      </c>
-      <c r="H2" t="s" s="4">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s" s="4">
-        <v>40</v>
-      </c>
-      <c r="J2" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="K2" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="L2" t="s" s="2">
+      <c r="P2" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="Q2" t="s" s="5">
+        <v>38</v>
+      </c>
+      <c r="R2" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="S2" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="T2" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="M2" t="s" s="2">
+      <c r="U2" t="s" s="2">
         <v>37</v>
-      </c>
-      <c r="N2" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="O2" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P2" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="Q2" t="s" s="4">
-        <v>39</v>
-      </c>
-      <c r="R2" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="S2" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T2" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="U2" t="s" s="4">
-        <v>39</v>
       </c>
       <c r="V2" t="s" s="2">
         <v>37</v>
@@ -802,25 +1031,25 @@
         <v>37</v>
       </c>
       <c r="X2" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="Y2" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="Z2" t="s" s="4">
+        <v>43</v>
+      </c>
+      <c r="Y2" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="Z2" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA2" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="AB2" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="AA2" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB2" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC2" t="s" s="6">
+      <c r="AC2" t="s" s="7">
         <v>45</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15.0" customHeight="true">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -830,17 +1059,17 @@
       <c r="C3" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="D3" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s" s="4">
-        <v>39</v>
+      <c r="D3" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>40</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H3" t="s" s="5">
         <v>38</v>
@@ -849,67 +1078,67 @@
         <v>39</v>
       </c>
       <c r="J3" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="K3" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="L3" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="M3" t="s" s="5">
+        <v>43</v>
+      </c>
+      <c r="K3" t="s" s="5">
         <v>38</v>
       </c>
-      <c r="N3" t="s" s="4">
+      <c r="L3" t="s" s="4">
         <v>39</v>
       </c>
+      <c r="M3" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="N3" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="O3" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="P3" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="Q3" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R3" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S3" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="T3" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="U3" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="V3" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="W3" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="X3" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y3" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="Z3" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA3" t="s" s="2">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="Z3" t="s" s="5">
+        <v>38</v>
+      </c>
+      <c r="AA3" t="s" s="4">
+        <v>39</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" ht="15.0" customHeight="true">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -917,191 +1146,191 @@
         <v>39</v>
       </c>
       <c r="C4" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I4" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K4" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="L4" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="M4" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="N4" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s" s="7">
         <v>45</v>
       </c>
-      <c r="O4" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P4" t="s" s="4">
-        <v>41</v>
-      </c>
-      <c r="Q4" t="s" s="5">
+      <c r="M4" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="N4" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="O4" t="s" s="6">
+        <v>46</v>
+      </c>
+      <c r="P4" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q4" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="R4" t="s" s="5">
         <v>38</v>
       </c>
-      <c r="R4" t="s" s="4">
+      <c r="S4" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="S4" t="s" s="2">
-        <v>37</v>
-      </c>
       <c r="T4" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U4" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="V4" t="s" s="4">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="U4" t="s" s="6">
+        <v>46</v>
+      </c>
+      <c r="V4" t="s" s="2">
+        <v>40</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="X4" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y4" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z4" t="s" s="2">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AB4" t="s" s="7">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AC4" t="s" s="4">
         <v>39</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15.0" customHeight="true">
       <c r="A5" t="s">
         <v>31</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="D5" t="s" s="5">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s" s="4">
+        <v>39</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="G5" t="s" s="5">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="G5" t="s" s="7">
+        <v>45</v>
       </c>
       <c r="H5" t="s" s="4">
         <v>39</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J5" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L5" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M5" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N5" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O5" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P5" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q5" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R5" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="S5" t="s" s="4">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="S5" t="s" s="2">
+        <v>40</v>
       </c>
       <c r="T5" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="U5" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="V5" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W5" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X5" t="s" s="5">
+        <v>40</v>
+      </c>
+      <c r="W5" t="s" s="5">
         <v>38</v>
       </c>
-      <c r="Y5" t="s" s="4">
+      <c r="X5" t="s" s="4">
         <v>39</v>
       </c>
+      <c r="Y5" t="s" s="3">
+        <v>43</v>
+      </c>
       <c r="Z5" t="s" s="2">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AA5" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB5" t="s" s="6">
-        <v>45</v>
-      </c>
-      <c r="AC5" t="s" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>40</v>
+      </c>
+      <c r="AB5" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC5" t="s" s="6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" ht="15.0" customHeight="true">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s" s="4">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="E6" t="s" s="2">
+        <v>40</v>
       </c>
       <c r="F6" t="s" s="5">
         <v>38</v>
@@ -1109,11 +1338,11 @@
       <c r="G6" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="H6" t="s" s="2">
-        <v>37</v>
+      <c r="H6" t="s" s="4">
+        <v>42</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J6" t="s" s="5">
         <v>38</v>
@@ -1122,34 +1351,34 @@
         <v>39</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="N6" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="N6" t="s" s="6">
+        <v>46</v>
       </c>
       <c r="O6" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="P6" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="Q6" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R6" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S6" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="T6" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="U6" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="V6" t="s" s="5">
         <v>38</v>
@@ -1158,119 +1387,119 @@
         <v>39</v>
       </c>
       <c r="X6" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y6" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="Z6" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="AA6" t="s" s="4">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="Z6" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA6" t="s" s="2">
+        <v>40</v>
       </c>
       <c r="AB6" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AC6" t="s" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" ht="15.0" customHeight="true">
       <c r="A7" t="s">
         <v>33</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I7" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J7" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K7" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="L7" t="s" s="5">
+        <v>43</v>
+      </c>
+      <c r="L7" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="M7" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="N7" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="O7" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P7" t="s" s="5">
         <v>38</v>
       </c>
-      <c r="M7" t="s" s="4">
+      <c r="Q7" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="N7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="O7" t="s" s="5">
+      <c r="R7" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="S7" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T7" t="s" s="5">
         <v>38</v>
       </c>
-      <c r="P7" t="s" s="4">
+      <c r="U7" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="Q7" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="R7" t="s" s="5">
+      <c r="V7" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W7" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X7" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="Y7" t="s" s="5">
         <v>38</v>
       </c>
-      <c r="S7" t="s" s="4">
+      <c r="Z7" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="T7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X7" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="Y7" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="Z7" t="s" s="2">
-        <v>37</v>
-      </c>
       <c r="AA7" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AB7" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AC7" t="s" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" ht="15.0" customHeight="true">
       <c r="A8" t="s">
         <v>34</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s" s="5">
         <v>38</v>
@@ -1279,182 +1508,182 @@
         <v>39</v>
       </c>
       <c r="E8" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="G8" t="s" s="2">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="G8" t="s" s="6">
+        <v>46</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="I8" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J8" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K8" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L8" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M8" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N8" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O8" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P8" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q8" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R8" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="S8" t="s" s="5">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="S8" t="s" s="7">
+        <v>45</v>
       </c>
       <c r="T8" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="U8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V8" t="s" s="2">
-        <v>37</v>
+      <c r="U8" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="V8" t="s" s="4">
+        <v>39</v>
       </c>
       <c r="W8" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="X8" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y8" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA8" t="s" s="6">
-        <v>45</v>
-      </c>
-      <c r="AB8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC8" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="AA8" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB8" t="s" s="6">
         <v>46</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="AC8" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" ht="15.0" customHeight="true">
       <c r="A9" t="s">
         <v>35</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G9" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H9" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I9" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J9" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="K9" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="L9" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="M9" t="s" s="5">
+        <v>38</v>
+      </c>
+      <c r="N9" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="O9" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="P9" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="Q9" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="R9" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="S9" t="s" s="6">
+        <v>46</v>
+      </c>
+      <c r="T9" t="s" s="4">
         <v>42</v>
       </c>
-      <c r="D9" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="E9" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="F9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I9" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J9" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="K9" t="s" s="5">
+      <c r="U9" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V9" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W9" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X9" t="s" s="5">
         <v>38</v>
       </c>
-      <c r="L9" t="s" s="4">
+      <c r="Y9" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="M9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="N9" t="s" s="7">
+      <c r="Z9" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA9" t="s" s="6">
         <v>46</v>
       </c>
-      <c r="O9" t="s" s="4">
-        <v>39</v>
-      </c>
-      <c r="P9" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Q9" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="R9" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="S9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T9" t="s" s="6">
-        <v>45</v>
-      </c>
-      <c r="U9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W9" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="X9" t="s" s="4">
-        <v>39</v>
-      </c>
-      <c r="Y9" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="Z9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA9" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="AB9" t="s" s="4">
-        <v>39</v>
+      <c r="AB9" t="s" s="2">
+        <v>40</v>
       </c>
       <c r="AC9" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" ht="15.0" customHeight="true">
       <c r="A10" t="s">
         <v>36</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s" s="5">
         <v>38</v>
@@ -1463,10 +1692,10 @@
         <v>39</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I10" t="s" s="5">
         <v>38</v>
@@ -1475,69 +1704,69 @@
         <v>39</v>
       </c>
       <c r="K10" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="N10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="O10" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="N10" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="O10" t="s" s="4">
+        <v>39</v>
       </c>
       <c r="P10" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="Q10" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R10" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S10" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T10" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="U10" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V10" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W10" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="X10" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y10" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z10" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AA10" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AB10" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AC10" t="s" s="4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" ht="15.0" customHeight="true">
       <c r="A12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0.0</v>
+        <v>48</v>
+      </c>
+      <c r="B12" t="n" s="15">
+        <v>0.19999999999999996</v>
       </c>
       <c r="C12" t="n">
         <v>1.0</v>
@@ -1552,11 +1781,11 @@
         <v>0.0</v>
       </c>
       <c r="G12" t="n" s="13">
+        <v>-1.0</v>
+      </c>
+      <c r="H12" t="n" s="13">
         <v>-0.6000000000000001</v>
       </c>
-      <c r="H12" t="n" s="13">
-        <v>-1.0</v>
-      </c>
       <c r="I12" t="n">
         <v>0.0</v>
       </c>
@@ -1569,61 +1798,61 @@
       <c r="L12" t="n">
         <v>0.0</v>
       </c>
-      <c r="M12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O12" t="n" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0.0</v>
+      <c r="M12" t="n" s="15">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="N12" t="n" s="15">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P12" t="n" s="15">
+        <v>0.6000000000000001</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="R12" t="n">
         <v>0.0</v>
       </c>
       <c r="S12" t="n" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="T12" t="n">
-        <v>0.0</v>
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="T12" t="n" s="15">
+        <v>1.2</v>
       </c>
       <c r="U12" t="n" s="15">
-        <v>1.0</v>
+        <v>1.2</v>
       </c>
       <c r="V12" t="n" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="W12" t="n">
-        <v>0.0</v>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="W12" t="n" s="15">
+        <v>0.20000000000000018</v>
       </c>
       <c r="X12" t="n">
         <v>0.0</v>
       </c>
       <c r="Y12" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Z12" t="n" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="AA12" t="n" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="AB12" t="n" s="15">
-        <v>1.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="Z12" t="n" s="17">
+        <v>2.2</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0.0</v>
       </c>
       <c r="AC12" t="n" s="15">
         <v>1.0</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" ht="15.0" customHeight="true">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B13" t="n">
         <v>0.0</v>
@@ -1632,10 +1861,10 @@
         <v>0.0</v>
       </c>
       <c r="D13" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E13" t="n" s="13">
-        <v>-1.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0</v>
       </c>
       <c r="F13" t="n">
         <v>0.0</v>
@@ -1653,56 +1882,56 @@
         <v>0.0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="L13" t="n" s="13">
+        <v>-1.0</v>
       </c>
       <c r="M13" t="n">
         <v>0.0</v>
       </c>
-      <c r="N13" t="n" s="13">
+      <c r="N13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA13" t="n" s="13">
         <v>-1.0</v>
       </c>
-      <c r="O13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="S13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="V13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="X13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>0.0</v>
-      </c>
       <c r="AB13" t="n">
         <v>0.0</v>
       </c>
@@ -1710,9 +1939,9 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" ht="15.0" customHeight="true">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B14" t="n" s="13">
         <v>-1.0</v>
@@ -1727,7 +1956,7 @@
         <v>-1.6</v>
       </c>
       <c r="F14" t="n" s="13">
-        <v>-1.0</v>
+        <v>-0.6000000000000001</v>
       </c>
       <c r="G14" t="n" s="13">
         <v>-1.0</v>
@@ -1742,7 +1971,7 @@
         <v>0.0</v>
       </c>
       <c r="K14" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L14" t="n">
         <v>0.0</v>
@@ -1756,76 +1985,76 @@
       <c r="O14" t="n">
         <v>0.0</v>
       </c>
-      <c r="P14" t="n" s="13">
+      <c r="P14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U14" t="n" s="13">
         <v>-0.6000000000000001</v>
       </c>
-      <c r="Q14" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="R14" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T14" t="n" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="U14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="V14" t="n" s="13">
+      <c r="V14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Z14" t="n" s="13">
+        <v>-0.6000000000000001</v>
+      </c>
+      <c r="AA14" t="n" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC14" t="n" s="13">
         <v>-1.0</v>
       </c>
-      <c r="W14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="X14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Z14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AA14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AB14" t="n" s="13">
+    </row>
+    <row r="15" ht="15.0" customHeight="true">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="n" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n" s="13">
         <v>-1.0</v>
       </c>
-      <c r="AC14" t="n" s="13">
-        <v>-0.6000000000000001</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="n" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.0</v>
+      <c r="H15" t="n" s="13">
+        <v>-1.0</v>
       </c>
       <c r="I15" t="n" s="13">
-        <v>-0.7999999999999998</v>
+        <v>-1.0</v>
       </c>
       <c r="J15" t="n">
         <v>1.0</v>
@@ -1854,8 +2083,8 @@
       <c r="R15" t="n">
         <v>0.0</v>
       </c>
-      <c r="S15" t="n">
-        <v>0.0</v>
+      <c r="S15" t="n" s="15">
+        <v>1.0</v>
       </c>
       <c r="T15" t="n">
         <v>0.0</v>
@@ -1870,16 +2099,16 @@
         <v>-1.0</v>
       </c>
       <c r="X15" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y15" t="n">
         <v>0.0</v>
       </c>
       <c r="Z15" t="n" s="13">
-        <v>-0.7999999999999998</v>
-      </c>
-      <c r="AA15" t="n" s="13">
-        <v>-0.8</v>
+        <v>-1.0</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>0.0</v>
       </c>
       <c r="AB15" t="n">
         <v>0.0</v>
@@ -1888,9 +2117,9 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="15.0" customHeight="true">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" t="n">
         <v>0.0</v>
@@ -1928,11 +2157,11 @@
       <c r="M16" t="n">
         <v>0.0</v>
       </c>
-      <c r="N16" t="n" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0.0</v>
+      <c r="N16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O16" t="n" s="13">
+        <v>-1.0</v>
       </c>
       <c r="P16" t="n">
         <v>0.0</v>
@@ -1977,12 +2206,12 @@
         <v>-1.0</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" ht="15.0" customHeight="true">
       <c r="A17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" t="n" s="27">
-        <v>0.0</v>
+        <v>43</v>
+      </c>
+      <c r="B17" t="n" s="23">
+        <v>0.19999999999999996</v>
       </c>
       <c r="C17" t="n" s="27">
         <v>1.0</v>
@@ -1991,79 +2220,79 @@
         <v>1.0</v>
       </c>
       <c r="E17" t="n" s="20">
-        <v>-3.6</v>
+        <v>-2.6</v>
       </c>
       <c r="F17" t="n" s="21">
+        <v>-1.6</v>
+      </c>
+      <c r="G17" t="n" s="21">
         <v>-2.0</v>
       </c>
-      <c r="G17" t="n" s="22">
-        <v>-0.6000000000000001</v>
-      </c>
-      <c r="H17" t="n" s="21">
+      <c r="H17" t="n" s="20">
+        <v>-2.6</v>
+      </c>
+      <c r="I17" t="n" s="20">
+        <v>-2.6</v>
+      </c>
+      <c r="J17" t="n" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="K17" t="n" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="L17" t="n" s="22">
+        <v>-1.0</v>
+      </c>
+      <c r="M17" t="n" s="22">
+        <v>-0.3999999999999999</v>
+      </c>
+      <c r="N17" t="n" s="22">
+        <v>-0.3999999999999999</v>
+      </c>
+      <c r="O17" t="n" s="21">
         <v>-2.0</v>
       </c>
-      <c r="I17" t="n" s="20">
-        <v>-2.4</v>
-      </c>
-      <c r="J17" t="n" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="K17" t="n" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="L17" t="n" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="M17" t="n" s="22">
+      <c r="P17" t="n" s="23">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="Q17" t="n" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="R17" t="n" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="S17" t="n" s="23">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="T17" t="n" s="23">
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="U17" t="n" s="23">
+        <v>0.5999999999999999</v>
+      </c>
+      <c r="V17" t="n" s="22">
+        <v>-0.8</v>
+      </c>
+      <c r="W17" t="n" s="21">
+        <v>-1.7999999999999998</v>
+      </c>
+      <c r="X17" t="n" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="Y17" t="n" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="Z17" t="n" s="22">
+        <v>-0.3999999999999999</v>
+      </c>
+      <c r="AA17" t="n" s="22">
         <v>-1.0</v>
       </c>
-      <c r="N17" t="n" s="22">
+      <c r="AB17" t="n" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="AC17" t="n" s="22">
         <v>-1.0</v>
-      </c>
-      <c r="O17" t="n" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="P17" t="n" s="22">
-        <v>-0.6000000000000001</v>
-      </c>
-      <c r="Q17" t="n" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="R17" t="n" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="S17" t="n" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="T17" t="n" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="U17" t="n" s="23">
-        <v>1.0</v>
-      </c>
-      <c r="V17" t="n" s="22">
-        <v>-1.0</v>
-      </c>
-      <c r="W17" t="n" s="21">
-        <v>-2.0</v>
-      </c>
-      <c r="X17" t="n" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="Y17" t="n" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="Z17" t="n" s="22">
-        <v>-0.7999999999999998</v>
-      </c>
-      <c r="AA17" t="n" s="22">
-        <v>-0.8</v>
-      </c>
-      <c r="AB17" t="n" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="AC17" t="n" s="22">
-        <v>-0.6000000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2082,81 +2311,78 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="U1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="W1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="X1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Y1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Z1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2165,81 +2391,78 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="E2" t="s">
         <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>44.0</v>
       </c>
       <c r="F2" t="s">
         <v>80</v>
       </c>
-      <c r="G2" t="s">
-        <v>81</v>
+      <c r="G2" t="n">
+        <v>1.0</v>
       </c>
       <c r="H2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I2" t="n">
         <v>6.0</v>
       </c>
-      <c r="J2" t="s">
-        <v>81</v>
+      <c r="I2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.4166666666666665</v>
       </c>
       <c r="K2" t="n">
-        <v>0.08333333333333348</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="L2" t="n">
-        <v>0.16666666666666663</v>
+        <v>160.0</v>
       </c>
       <c r="M2" t="n">
-        <v>160.0</v>
+        <v>120.0</v>
       </c>
       <c r="N2" t="n">
-        <v>120.0</v>
+        <v>132.0</v>
       </c>
       <c r="O2" t="n">
-        <v>132.0</v>
+        <v>121.5</v>
       </c>
       <c r="P2" t="n">
-        <v>125.0</v>
+        <v>40.5</v>
       </c>
       <c r="Q2" t="n">
-        <v>41.666666666666664</v>
+        <v>2.9166666666666665</v>
       </c>
       <c r="R2" t="n">
-        <v>2.9166666666666665</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="S2" t="n">
-        <v>0.8333333333333334</v>
+        <v>2.5</v>
       </c>
       <c r="T2" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="U2" t="n">
         <v>3.0</v>
       </c>
       <c r="V2" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="W2" t="n">
-        <v>1.0</v>
+        <v>14.0</v>
       </c>
       <c r="X2" t="n">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="Z2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="AA2" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2248,58 +2471,58 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" t="s">
         <v>79</v>
       </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>44.0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" t="s">
-        <v>80</v>
+      <c r="G3" t="n">
+        <v>1.0</v>
       </c>
       <c r="H3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I3" t="n">
         <v>7.0</v>
       </c>
-      <c r="J3" t="s">
-        <v>80</v>
+      <c r="I3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.11111111111111116</v>
       </c>
       <c r="K3" t="n">
-        <v>0.11111111111111116</v>
+        <v>-0.11111111111111116</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.11111111111111116</v>
+        <v>160.0</v>
       </c>
       <c r="M3" t="n">
         <v>160.0</v>
       </c>
       <c r="N3" t="n">
-        <v>160.0</v>
+        <v>176.0</v>
       </c>
       <c r="O3" t="n">
-        <v>176.0</v>
+        <v>170.0</v>
       </c>
       <c r="P3" t="n">
-        <v>170.0</v>
+        <v>42.5</v>
       </c>
       <c r="Q3" t="n">
-        <v>42.5</v>
+        <v>3.888888888888889</v>
       </c>
       <c r="R3" t="n">
-        <v>3.888888888888889</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="S3" t="n">
-        <v>1.1111111111111112</v>
+        <v>4.0</v>
       </c>
       <c r="T3" t="n">
         <v>4.0</v>
@@ -2308,22 +2531,19 @@
         <v>4.0</v>
       </c>
       <c r="V3" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="W3" t="n">
         <v>1.0</v>
       </c>
       <c r="X3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="Z3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -2331,58 +2551,58 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="E4" t="s">
         <v>79</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>44.0</v>
       </c>
       <c r="F4" t="s">
         <v>80</v>
       </c>
-      <c r="G4" t="s">
-        <v>81</v>
+      <c r="G4" t="n">
+        <v>1.0</v>
       </c>
       <c r="H4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I4" t="n">
         <v>7.0</v>
       </c>
-      <c r="J4" t="s">
-        <v>81</v>
+      <c r="I4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.08333333333333348</v>
       </c>
       <c r="K4" t="n">
-        <v>0.08333333333333348</v>
+        <v>-0.2333333333333334</v>
       </c>
       <c r="L4" t="n">
-        <v>0.16666666666666663</v>
+        <v>160.0</v>
       </c>
       <c r="M4" t="n">
-        <v>160.0</v>
+        <v>120.0</v>
       </c>
       <c r="N4" t="n">
-        <v>120.0</v>
+        <v>132.0</v>
       </c>
       <c r="O4" t="n">
-        <v>132.0</v>
+        <v>121.0</v>
       </c>
       <c r="P4" t="n">
-        <v>124.0</v>
+        <v>40.333333333333336</v>
       </c>
       <c r="Q4" t="n">
-        <v>41.333333333333336</v>
+        <v>2.9166666666666665</v>
       </c>
       <c r="R4" t="n">
-        <v>2.9166666666666665</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="S4" t="n">
-        <v>0.8333333333333334</v>
+        <v>3.0</v>
       </c>
       <c r="T4" t="n">
         <v>3.0</v>
@@ -2391,22 +2611,19 @@
         <v>3.0</v>
       </c>
       <c r="V4" t="n">
-        <v>3.0</v>
+        <v>0.6</v>
       </c>
       <c r="W4" t="n">
-        <v>1.0</v>
+        <v>15.0</v>
       </c>
       <c r="X4" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="Z4" t="n">
         <v>0.0</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>1.0</v>
       </c>
     </row>
     <row r="5">
@@ -2414,81 +2631,78 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="E5" t="s">
         <v>79</v>
-      </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>44.0</v>
       </c>
       <c r="F5" t="s">
         <v>80</v>
       </c>
-      <c r="G5" t="s">
-        <v>81</v>
+      <c r="G5" t="n">
+        <v>1.0</v>
       </c>
       <c r="H5" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I5" t="n">
         <v>6.0</v>
       </c>
-      <c r="J5" t="s">
-        <v>81</v>
+      <c r="I5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.08333333333333348</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.4166666666666665</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="L5" t="n">
-        <v>0.16666666666666663</v>
+        <v>160.0</v>
       </c>
       <c r="M5" t="n">
-        <v>160.0</v>
+        <v>120.0</v>
       </c>
       <c r="N5" t="n">
-        <v>120.0</v>
+        <v>132.0</v>
       </c>
       <c r="O5" t="n">
-        <v>132.0</v>
+        <v>125.0</v>
       </c>
       <c r="P5" t="n">
-        <v>120.5</v>
+        <v>41.666666666666664</v>
       </c>
       <c r="Q5" t="n">
-        <v>40.166666666666664</v>
+        <v>2.9166666666666665</v>
       </c>
       <c r="R5" t="n">
-        <v>2.9166666666666665</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="S5" t="n">
-        <v>0.8333333333333334</v>
+        <v>3.0</v>
       </c>
       <c r="T5" t="n">
-        <v>2.5</v>
+        <v>3.0</v>
       </c>
       <c r="U5" t="n">
         <v>3.0</v>
       </c>
       <c r="V5" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="W5" t="n">
-        <v>1.0</v>
+        <v>13.0</v>
       </c>
       <c r="X5" t="n">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y5" t="n">
         <v>0.0</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AA5" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2497,81 +2711,78 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="E6" t="s">
         <v>79</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>44.0</v>
       </c>
       <c r="F6" t="s">
         <v>80</v>
       </c>
-      <c r="G6" t="s">
-        <v>81</v>
+      <c r="G6" t="n">
+        <v>1.0</v>
       </c>
       <c r="H6" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I6" t="n">
         <v>7.0</v>
       </c>
-      <c r="J6" t="s">
-        <v>81</v>
+      <c r="I6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-0.19444444444444464</v>
       </c>
       <c r="K6" t="n">
-        <v>0.30555555555555536</v>
+        <v>-0.05555555555555558</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.05555555555555558</v>
+        <v>160.0</v>
       </c>
       <c r="M6" t="n">
-        <v>160.0</v>
+        <v>152.0</v>
       </c>
       <c r="N6" t="n">
-        <v>152.0</v>
+        <v>167.20000000000002</v>
       </c>
       <c r="O6" t="n">
-        <v>167.20000000000002</v>
+        <v>152.5</v>
       </c>
       <c r="P6" t="n">
-        <v>160.0</v>
+        <v>40.13157894736842</v>
       </c>
       <c r="Q6" t="n">
-        <v>42.10526315789474</v>
+        <v>3.6944444444444446</v>
       </c>
       <c r="R6" t="n">
-        <v>3.6944444444444446</v>
+        <v>1.0555555555555556</v>
       </c>
       <c r="S6" t="n">
-        <v>1.0555555555555556</v>
+        <v>3.5</v>
       </c>
       <c r="T6" t="n">
         <v>4.0</v>
       </c>
       <c r="U6" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="V6" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="W6" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="X6" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="Z6" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="AA6" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -2580,58 +2791,58 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="C7" t="n">
+        <v>40.0</v>
       </c>
       <c r="D7" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="E7" t="n">
         <v>44.0</v>
       </c>
+      <c r="E7" t="s">
+        <v>80</v>
+      </c>
       <c r="F7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.0</v>
       </c>
       <c r="H7" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I7" t="n">
         <v>7.0</v>
       </c>
-      <c r="J7" t="s">
-        <v>81</v>
+      <c r="I7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.08333333333333348</v>
       </c>
       <c r="K7" t="n">
-        <v>0.08333333333333348</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.2333333333333334</v>
+        <v>160.0</v>
       </c>
       <c r="M7" t="n">
-        <v>160.0</v>
+        <v>120.0</v>
       </c>
       <c r="N7" t="n">
-        <v>120.0</v>
+        <v>132.0</v>
       </c>
       <c r="O7" t="n">
-        <v>132.0</v>
+        <v>130.0</v>
       </c>
       <c r="P7" t="n">
-        <v>125.0</v>
+        <v>43.333333333333336</v>
       </c>
       <c r="Q7" t="n">
-        <v>41.666666666666664</v>
+        <v>2.9166666666666665</v>
       </c>
       <c r="R7" t="n">
-        <v>2.9166666666666665</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="S7" t="n">
-        <v>0.8333333333333334</v>
+        <v>3.0</v>
       </c>
       <c r="T7" t="n">
         <v>3.0</v>
@@ -2640,21 +2851,18 @@
         <v>3.0</v>
       </c>
       <c r="V7" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="W7" t="n">
-        <v>0.6</v>
+        <v>10.0</v>
       </c>
       <c r="X7" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y7" t="n">
         <v>0.0</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AA7" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2663,58 +2871,58 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="E8" t="s">
         <v>79</v>
       </c>
-      <c r="C8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" t="n">
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.2777777777777777</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="L8" t="n">
+        <v>160.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>112.0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>123.20000000000002</v>
+      </c>
+      <c r="O8" t="n">
+        <v>112.0</v>
+      </c>
+      <c r="P8" t="n">
         <v>40.0</v>
       </c>
-      <c r="E8" t="n">
-        <v>44.0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>81</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.2777777777777777</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.2222222222222222</v>
-      </c>
-      <c r="M8" t="n">
-        <v>160.0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>112.0</v>
-      </c>
-      <c r="O8" t="n">
-        <v>123.20000000000002</v>
-      </c>
-      <c r="P8" t="n">
-        <v>113.0</v>
-      </c>
       <c r="Q8" t="n">
-        <v>40.357142857142854</v>
+        <v>2.7222222222222223</v>
       </c>
       <c r="R8" t="n">
-        <v>2.7222222222222223</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="S8" t="n">
-        <v>0.7777777777777778</v>
+        <v>3.0</v>
       </c>
       <c r="T8" t="n">
         <v>3.0</v>
@@ -2723,21 +2931,18 @@
         <v>3.0</v>
       </c>
       <c r="V8" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="W8" t="n">
-        <v>1.0</v>
+        <v>12.0</v>
       </c>
       <c r="X8" t="n">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y8" t="n">
         <v>0.0</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AA8" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2746,81 +2951,78 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="E9" t="s">
         <v>79</v>
-      </c>
-      <c r="C9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>44.0</v>
       </c>
       <c r="F9" t="s">
         <v>80</v>
       </c>
-      <c r="G9" t="s">
-        <v>81</v>
+      <c r="G9" t="n">
+        <v>1.0</v>
       </c>
       <c r="H9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I9" t="n">
         <v>7.0</v>
       </c>
-      <c r="J9" t="s">
-        <v>81</v>
+      <c r="I9" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-0.38888888888888884</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.38888888888888884</v>
+        <v>-0.11111111111111116</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.11111111111111116</v>
+        <v>160.0</v>
       </c>
       <c r="M9" t="n">
         <v>160.0</v>
       </c>
       <c r="N9" t="n">
-        <v>160.0</v>
+        <v>176.0</v>
       </c>
       <c r="O9" t="n">
-        <v>176.0</v>
+        <v>160.5</v>
       </c>
       <c r="P9" t="n">
-        <v>160.5</v>
+        <v>40.125</v>
       </c>
       <c r="Q9" t="n">
-        <v>40.125</v>
+        <v>3.888888888888889</v>
       </c>
       <c r="R9" t="n">
-        <v>3.888888888888889</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="S9" t="n">
-        <v>1.1111111111111112</v>
+        <v>3.5</v>
       </c>
       <c r="T9" t="n">
-        <v>3.5</v>
+        <v>4.0</v>
       </c>
       <c r="U9" t="n">
         <v>3.0</v>
       </c>
       <c r="V9" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="W9" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="X9" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y9" t="n">
         <v>0.0</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AA9" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2829,81 +3031,78 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="E10" t="s">
         <v>79</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>44.0</v>
       </c>
       <c r="F10" t="s">
         <v>80</v>
       </c>
-      <c r="G10" t="s">
-        <v>81</v>
+      <c r="G10" t="n">
+        <v>1.0</v>
       </c>
       <c r="H10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I10" t="n">
         <v>7.0</v>
       </c>
-      <c r="J10" t="s">
-        <v>80</v>
+      <c r="I10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.36111111111111116</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.13888888888888884</v>
+        <v>-0.21111111111111114</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.21111111111111114</v>
+        <v>160.0</v>
       </c>
       <c r="M10" t="n">
-        <v>160.0</v>
+        <v>88.0</v>
       </c>
       <c r="N10" t="n">
-        <v>88.0</v>
+        <v>96.80000000000001</v>
       </c>
       <c r="O10" t="n">
-        <v>96.80000000000001</v>
+        <v>92.5</v>
       </c>
       <c r="P10" t="n">
-        <v>90.0</v>
+        <v>42.04545454545455</v>
       </c>
       <c r="Q10" t="n">
-        <v>40.90909090909091</v>
+        <v>2.138888888888889</v>
       </c>
       <c r="R10" t="n">
-        <v>2.138888888888889</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="S10" t="n">
-        <v>0.6111111111111112</v>
+        <v>2.5</v>
       </c>
       <c r="T10" t="n">
         <v>2.0</v>
       </c>
       <c r="U10" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="V10" t="n">
-        <v>2.0</v>
+        <v>0.4</v>
       </c>
       <c r="W10" t="n">
-        <v>0.4</v>
+        <v>18.0</v>
       </c>
       <c r="X10" t="n">
-        <v>18.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y10" t="n">
         <v>0.0</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AA10" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2923,42 +3122,42 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
         <v>82</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>83</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>84</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>85</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>86</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>87</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>88</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>89</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>90</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>91</v>
-      </c>
-      <c r="L1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="n">
         <v>0.0</v>
@@ -2973,7 +3172,7 @@
         <v>5.0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7222222222222219</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G2" t="n">
         <v>0.4555555555555556</v>
@@ -2985,13 +3184,435 @@
         <v>16.0</v>
       </c>
       <c r="J2" t="n">
-        <v>5.0</v>
+        <v>9.0</v>
       </c>
       <c r="K2" t="n">
-        <v>29.4</v>
+        <v>30.6</v>
       </c>
       <c r="L2" t="n">
-        <v>28.92</v>
+        <v>30.360000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="2" max="2" width="56.51953125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed small formatting error
</commit_message>
<xml_diff>
--- a/example/schedule.xlsx
+++ b/example/schedule.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="102">
   <si>
     <t>01</t>
   </si>
@@ -128,39 +128,36 @@
     <t>Cottle</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>FT</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>N2</t>
   </si>
   <si>
     <t>N1</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>4_2</t>
   </si>
   <si>
@@ -308,6 +305,9 @@
     <t>4</t>
   </si>
   <si>
+    <t>2019-02-07: No split possible based on provisional day presence</t>
+  </si>
+  <si>
     <t>2019-02-08: No split possible based on provisional day presence</t>
   </si>
   <si>
@@ -317,16 +317,10 @@
     <t>2019-02-04: No split possible based on provisional day presence</t>
   </si>
   <si>
-    <t>2019-02-07: No split possible based on provisional day presence</t>
-  </si>
-  <si>
     <t>2019-02-05: No split possible based on provisional day presence</t>
   </si>
   <si>
     <t>2019-02-12: No split possible based on provisional day presence</t>
-  </si>
-  <si>
-    <t>Unable to assign FT for Crusher in this week, trying next week...</t>
   </si>
 </sst>
 </file>
@@ -675,7 +669,7 @@
   <sheetData>
     <row r="1" ht="15.0" customHeight="true">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -766,59 +760,59 @@
       <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" t="s" s="5">
         <v>37</v>
       </c>
-      <c r="C2" t="s" s="3">
-        <v>44</v>
+      <c r="C2" t="s" s="4">
+        <v>39</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J2" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K2" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="L2" t="s" s="6">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="L2" t="s" s="2">
+        <v>38</v>
       </c>
       <c r="M2" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="N2" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="O2" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="P2" t="s" s="5">
         <v>37</v>
       </c>
-      <c r="N2" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="O2" t="s" s="4">
-        <v>42</v>
-      </c>
-      <c r="P2" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Q2" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="R2" t="s" s="4">
+      <c r="Q2" t="s" s="4">
         <v>39</v>
       </c>
+      <c r="R2" t="s" s="3">
+        <v>42</v>
+      </c>
       <c r="S2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T2" t="s" s="7">
         <v>45</v>
@@ -827,25 +821,25 @@
         <v>39</v>
       </c>
       <c r="V2" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="W2" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="X2" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Y2" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="Z2" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="AA2" t="s" s="4">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="Z2" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA2" t="s" s="2">
+        <v>38</v>
       </c>
       <c r="AB2" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC2" t="s" s="6">
         <v>46</v>
@@ -855,89 +849,89 @@
       <c r="A3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s" s="4">
-        <v>39</v>
+      <c r="B3" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s" s="3">
+        <v>42</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="F3" t="s" s="4">
-        <v>42</v>
+      <c r="F3" t="s" s="2">
+        <v>38</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s" s="5">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s" s="4">
         <v>39</v>
       </c>
       <c r="J3" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K3" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N3" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O3" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P3" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Q3" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R3" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S3" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T3" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="U3" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V3" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="W3" t="s" s="4">
+        <v>38</v>
+      </c>
+      <c r="V3" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W3" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="X3" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="X3" t="s" s="3">
-        <v>44</v>
-      </c>
       <c r="Y3" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="Z3" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA3" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="Z3" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="AA3" t="s" s="4">
+        <v>39</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="true">
@@ -948,31 +942,31 @@
         <v>39</v>
       </c>
       <c r="C4" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K4" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L4" t="s" s="7">
         <v>45</v>
@@ -980,53 +974,53 @@
       <c r="M4" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="N4" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="O4" t="s" s="6">
+      <c r="N4" t="s" s="6">
         <v>46</v>
       </c>
-      <c r="P4" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Q4" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="R4" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="S4" t="s" s="4">
+      <c r="O4" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="P4" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="Q4" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="R4" t="s" s="4">
         <v>39</v>
       </c>
+      <c r="S4" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="T4" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U4" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="U4" t="s" s="6">
+        <v>46</v>
       </c>
       <c r="V4" t="s" s="2">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="X4" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Y4" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Z4" t="s" s="2">
         <v>43</v>
       </c>
-      <c r="AA4" t="s" s="6">
-        <v>46</v>
-      </c>
-      <c r="AB4" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC4" t="s" s="2">
-        <v>40</v>
+      <c r="AA4" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB4" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="AC4" t="s" s="4">
+        <v>39</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="true">
@@ -1034,19 +1028,19 @@
         <v>31</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s" s="2">
         <v>44</v>
-      </c>
-      <c r="D5" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F5" t="s" s="2">
-        <v>40</v>
       </c>
       <c r="G5" t="s" s="7">
         <v>45</v>
@@ -1055,67 +1049,67 @@
         <v>39</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="J5" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K5" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L5" t="s" s="4">
+        <v>40</v>
+      </c>
+      <c r="M5" t="s" s="4">
+        <v>40</v>
+      </c>
+      <c r="N5" t="s" s="4">
+        <v>40</v>
+      </c>
+      <c r="O5" t="s" s="4">
+        <v>40</v>
+      </c>
+      <c r="P5" t="s" s="4">
+        <v>40</v>
+      </c>
+      <c r="Q5" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="R5" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="S5" t="s" s="4">
         <v>41</v>
-      </c>
-      <c r="M5" t="s" s="4">
-        <v>41</v>
-      </c>
-      <c r="N5" t="s" s="4">
-        <v>41</v>
-      </c>
-      <c r="O5" t="s" s="4">
-        <v>41</v>
-      </c>
-      <c r="P5" t="s" s="4">
-        <v>41</v>
-      </c>
-      <c r="Q5" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="R5" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="S5" t="s" s="4">
-        <v>42</v>
       </c>
       <c r="T5" t="s" s="6">
         <v>46</v>
       </c>
       <c r="U5" t="s" s="2">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="V5" t="s" s="2">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="W5" t="s" s="2">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="X5" t="s" s="5">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y5" t="s" s="4">
         <v>39</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="AA5" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB5" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="AC5" t="s" s="4">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="AB5" t="s" s="6">
+        <v>46</v>
+      </c>
+      <c r="AC5" t="s" s="2">
+        <v>44</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="true">
@@ -1123,88 +1117,88 @@
         <v>32</v>
       </c>
       <c r="B6" t="s" s="4">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s" s="4">
         <v>41</v>
       </c>
-      <c r="C6" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="F6" t="s" s="5">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s" s="4">
         <v>39</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I6" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="J6" t="s" s="4">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J6" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="K6" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="K6" t="s" s="3">
-        <v>44</v>
-      </c>
       <c r="L6" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="N6" t="s" s="6">
+        <v>38</v>
+      </c>
+      <c r="N6" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="O6" t="s" s="6">
         <v>46</v>
       </c>
-      <c r="O6" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="P6" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Q6" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R6" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S6" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T6" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="U6" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V6" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W6" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="X6" t="s" s="4">
+        <v>38</v>
+      </c>
+      <c r="V6" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="W6" t="s" s="4">
         <v>39</v>
       </c>
+      <c r="X6" t="s" s="3">
+        <v>42</v>
+      </c>
       <c r="Y6" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Z6" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AB6" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC6" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="true">
@@ -1212,88 +1206,88 @@
         <v>33</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I7" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J7" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K7" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="M7" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="N7" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="M7" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="N7" t="s" s="4">
+        <v>39</v>
       </c>
       <c r="O7" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P7" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="Q7" t="s" s="4">
+        <v>38</v>
+      </c>
+      <c r="P7" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Q7" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="R7" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="S7" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="T7" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="R7" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="S7" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T7" t="s" s="4">
-        <v>47</v>
-      </c>
-      <c r="U7" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="V7" t="s" s="4">
-        <v>39</v>
+      <c r="U7" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V7" t="s" s="2">
+        <v>38</v>
       </c>
       <c r="W7" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="X7" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Y7" t="s" s="5">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Z7" t="s" s="4">
         <v>39</v>
       </c>
       <c r="AA7" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AB7" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC7" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="true">
@@ -1301,19 +1295,19 @@
         <v>34</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s" s="5">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s" s="4">
         <v>39</v>
       </c>
       <c r="E8" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s" s="6">
         <v>46</v>
@@ -1325,61 +1319,61 @@
         <v>43</v>
       </c>
       <c r="J8" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K8" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L8" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M8" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N8" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O8" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P8" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q8" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R8" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="S8" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="S8" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T8" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U8" t="s" s="7">
         <v>45</v>
       </c>
-      <c r="T8" t="s" s="4">
+      <c r="V8" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="U8" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V8" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="W8" t="s" s="2">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="X8" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Y8" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="Z8" t="s" s="6">
+        <v>42</v>
+      </c>
+      <c r="Z8" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA8" t="s" s="6">
         <v>46</v>
       </c>
-      <c r="AA8" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="AB8" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC8" t="s" s="7">
         <v>45</v>
@@ -1390,13 +1384,13 @@
         <v>35</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s" s="2">
         <v>43</v>
@@ -1407,26 +1401,26 @@
       <c r="G9" t="s" s="2">
         <v>43</v>
       </c>
-      <c r="H9" t="s" s="4">
-        <v>42</v>
-      </c>
-      <c r="I9" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J9" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="K9" t="s" s="4">
+      <c r="H9" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I9" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="J9" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="L9" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="M9" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="N9" t="s" s="4">
-        <v>39</v>
+      <c r="K9" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="L9" t="s" s="6">
+        <v>46</v>
+      </c>
+      <c r="M9" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="N9" t="s" s="2">
+        <v>38</v>
       </c>
       <c r="O9" t="s" s="7">
         <v>45</v>
@@ -1435,31 +1429,31 @@
         <v>39</v>
       </c>
       <c r="Q9" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="R9" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="S9" t="s" s="6">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="R9" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="S9" t="s" s="4">
+        <v>39</v>
       </c>
       <c r="T9" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="U9" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="V9" t="s" s="2">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="W9" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="X9" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Y9" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Z9" t="s" s="2">
         <v>43</v>
@@ -1471,7 +1465,7 @@
         <v>39</v>
       </c>
       <c r="AC9" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="true">
@@ -1479,40 +1473,40 @@
         <v>36</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s" s="5">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s" s="4">
         <v>39</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J10" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K10" t="s" s="5">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L10" t="s" s="4">
         <v>39</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N10" t="s" s="7">
         <v>45</v>
@@ -1521,54 +1515,54 @@
         <v>39</v>
       </c>
       <c r="P10" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Q10" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R10" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S10" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T10" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U10" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V10" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W10" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X10" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Y10" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Z10" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AA10" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AB10" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC10" t="s" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" ht="15.0" customHeight="true">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" t="n">
-        <v>0.19999999999999996</v>
+        <v>0.0</v>
       </c>
       <c r="C12" t="n">
         <v>1.0</v>
@@ -1580,7 +1574,7 @@
         <v>-1.0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="G12" t="n" s="13">
         <v>-1.0</v>
@@ -1601,37 +1595,37 @@
         <v>0.0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.19999999999999996</v>
+        <v>0.0</v>
       </c>
       <c r="N12" t="n">
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="O12" t="n" s="15">
+        <v>1.0</v>
       </c>
       <c r="P12" t="n">
-        <v>0.19999999999999996</v>
+        <v>0.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="R12" t="n">
         <v>0.0</v>
       </c>
-      <c r="S12" t="n">
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="T12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U12" t="n" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="V12" t="n" s="15">
-        <v>1.0</v>
+      <c r="S12" t="n" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="T12" t="n" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.0</v>
       </c>
       <c r="W12" t="n">
-        <v>0.3999999999999999</v>
+        <v>0.0</v>
       </c>
       <c r="X12" t="n">
         <v>0.0</v>
@@ -1639,11 +1633,11 @@
       <c r="Y12" t="n">
         <v>0.0</v>
       </c>
-      <c r="Z12" t="n" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>0.0</v>
+      <c r="Z12" t="n" s="17">
+        <v>2.0</v>
+      </c>
+      <c r="AA12" t="n" s="15">
+        <v>1.0</v>
       </c>
       <c r="AB12" t="n" s="15">
         <v>1.0</v>
@@ -1654,7 +1648,7 @@
     </row>
     <row r="13" ht="15.0" customHeight="true">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" t="n">
         <v>0.0</v>
@@ -1668,8 +1662,8 @@
       <c r="E13" t="n" s="13">
         <v>-1.0</v>
       </c>
-      <c r="F13" t="n" s="13">
-        <v>-1.0</v>
+      <c r="F13" t="n">
+        <v>0.0</v>
       </c>
       <c r="G13" t="n">
         <v>0.0</v>
@@ -1719,20 +1713,20 @@
       <c r="V13" t="n">
         <v>0.0</v>
       </c>
-      <c r="W13" t="n" s="13">
+      <c r="W13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA13" t="n" s="13">
         <v>-1.0</v>
-      </c>
-      <c r="X13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>0.0</v>
       </c>
       <c r="AB13" t="n">
         <v>0.0</v>
@@ -1743,10 +1737,10 @@
     </row>
     <row r="14" ht="15.0" customHeight="true">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" t="n" s="13">
-        <v>-0.6000000000000001</v>
+        <v>-1.0</v>
       </c>
       <c r="C14" t="n">
         <v>0.0</v>
@@ -1763,14 +1757,14 @@
       <c r="G14" t="n" s="13">
         <v>-0.6000000000000001</v>
       </c>
-      <c r="H14" t="n" s="11">
-        <v>-2.0</v>
+      <c r="H14" t="n" s="13">
+        <v>-1.0</v>
       </c>
       <c r="I14" t="n" s="13">
-        <v>-0.6000000000000001</v>
+        <v>-1.0</v>
       </c>
       <c r="J14" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K14" t="n">
         <v>0.0</v>
@@ -1787,11 +1781,11 @@
       <c r="O14" t="n">
         <v>0.0</v>
       </c>
-      <c r="P14" t="n">
-        <v>0.0</v>
+      <c r="P14" t="n" s="13">
+        <v>-1.0</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="R14" t="n">
         <v>1.0</v>
@@ -1805,8 +1799,8 @@
       <c r="U14" t="n">
         <v>0.0</v>
       </c>
-      <c r="V14" t="n" s="13">
-        <v>-0.20000000000000018</v>
+      <c r="V14" t="n">
+        <v>0.0</v>
       </c>
       <c r="W14" t="n">
         <v>0.0</v>
@@ -1823,16 +1817,16 @@
       <c r="AA14" t="n">
         <v>0.0</v>
       </c>
-      <c r="AB14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AC14" t="n">
-        <v>0.0</v>
+      <c r="AB14" t="n" s="13">
+        <v>-1.0</v>
+      </c>
+      <c r="AC14" t="n" s="13">
+        <v>-1.0</v>
       </c>
     </row>
     <row r="15" ht="15.0" customHeight="true">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" t="n" s="15">
         <v>1.0</v>
@@ -1843,11 +1837,11 @@
       <c r="D15" t="n">
         <v>0.0</v>
       </c>
-      <c r="E15" t="n" s="15">
-        <v>1.0</v>
+      <c r="E15" t="n">
+        <v>0.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0</v>
+        <v>0.20000000000000018</v>
       </c>
       <c r="G15" t="n" s="13">
         <v>-1.0</v>
@@ -1856,10 +1850,10 @@
         <v>0.0</v>
       </c>
       <c r="I15" t="n" s="13">
-        <v>-1.0</v>
+        <v>-0.7999999999999998</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K15" t="n">
         <v>0.0</v>
@@ -1892,13 +1886,13 @@
         <v>0.0</v>
       </c>
       <c r="U15" t="n">
-        <v>0.0</v>
+        <v>0.20000000000000018</v>
       </c>
       <c r="V15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W15" t="n">
-        <v>0.0</v>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="W15" t="n" s="13">
+        <v>-0.8</v>
       </c>
       <c r="X15" t="n">
         <v>1.0</v>
@@ -1907,21 +1901,21 @@
         <v>0.0</v>
       </c>
       <c r="Z15" t="n" s="13">
-        <v>-1.0</v>
+        <v>-0.7999999999999998</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.0</v>
+        <v>0.20000000000000018</v>
       </c>
       <c r="AB15" t="n">
         <v>0.0</v>
       </c>
-      <c r="AC15" t="n" s="13">
-        <v>-1.0</v>
+      <c r="AC15" t="n">
+        <v>0.20000000000000018</v>
       </c>
     </row>
     <row r="16" ht="15.0" customHeight="true">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" t="n">
         <v>0.0</v>
@@ -2010,10 +2004,10 @@
     </row>
     <row r="17" ht="15.0" customHeight="true">
       <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0.5999999999999999</v>
+        <v>42</v>
+      </c>
+      <c r="B17" t="n" s="27">
+        <v>0.0</v>
       </c>
       <c r="C17" t="n" s="27">
         <v>1.0</v>
@@ -2022,19 +2016,19 @@
         <v>1.0</v>
       </c>
       <c r="E17" t="n" s="20">
-        <v>-2.6</v>
-      </c>
-      <c r="F17" t="n" s="20">
-        <v>-2.6</v>
+        <v>-3.6</v>
+      </c>
+      <c r="F17" t="n" s="22">
+        <v>-1.0</v>
       </c>
       <c r="G17" t="n" s="21">
         <v>-1.6</v>
       </c>
-      <c r="H17" t="n" s="20">
-        <v>-2.6</v>
+      <c r="H17" t="n" s="21">
+        <v>-1.6</v>
       </c>
       <c r="I17" t="n" s="20">
-        <v>-2.2</v>
+        <v>-2.4</v>
       </c>
       <c r="J17" t="n" s="27">
         <v>1.0</v>
@@ -2046,55 +2040,55 @@
         <v>-1.0</v>
       </c>
       <c r="M17" t="n" s="22">
+        <v>-1.0</v>
+      </c>
+      <c r="N17" t="n" s="22">
+        <v>-1.0</v>
+      </c>
+      <c r="O17" t="n" s="22">
+        <v>-1.0</v>
+      </c>
+      <c r="P17" t="n" s="22">
+        <v>-1.0</v>
+      </c>
+      <c r="Q17" t="n" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="R17" t="n" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="S17" t="n" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="T17" t="n" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="U17" t="n" s="27">
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="V17" t="n" s="27">
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="W17" t="n" s="22">
         <v>-0.8</v>
       </c>
-      <c r="N17" t="n" s="22">
-        <v>-0.8</v>
-      </c>
-      <c r="O17" t="n" s="21">
-        <v>-2.0</v>
-      </c>
-      <c r="P17" t="n">
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="Q17" t="n" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="R17" t="n" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="S17" t="n">
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="T17" t="n" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="U17" t="n" s="23">
-        <v>1.0</v>
-      </c>
-      <c r="V17" t="n">
-        <v>0.7999999999999998</v>
-      </c>
-      <c r="W17" t="n" s="22">
-        <v>-0.6000000000000001</v>
-      </c>
       <c r="X17" t="n" s="27">
         <v>1.0</v>
       </c>
       <c r="Y17" t="n" s="27">
         <v>1.0</v>
       </c>
-      <c r="Z17" t="n" s="22">
-        <v>-0.20000000000000018</v>
+      <c r="Z17" t="n" s="23">
+        <v>1.0</v>
       </c>
       <c r="AA17" t="n" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="AB17" t="n" s="23">
-        <v>1.0</v>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="AB17" t="n" s="27">
+        <v>0.0</v>
       </c>
       <c r="AC17" t="n" s="27">
-        <v>0.0</v>
+        <v>0.20000000000000018</v>
       </c>
     </row>
   </sheetData>
@@ -2113,79 +2107,79 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>57</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>58</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>62</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>63</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>64</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>65</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>66</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>67</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>69</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>70</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>71</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>72</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>73</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>74</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>75</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>76</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>77</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2">
@@ -2193,7 +2187,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" t="n">
         <v>40.0</v>
@@ -2202,10 +2196,10 @@
         <v>44.0</v>
       </c>
       <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
         <v>79</v>
-      </c>
-      <c r="F2" t="s">
-        <v>80</v>
       </c>
       <c r="G2" t="n">
         <v>1.0</v>
@@ -2214,13 +2208,13 @@
         <v>6.0</v>
       </c>
       <c r="I2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J2" t="n">
         <v>0.08333333333333348</v>
       </c>
       <c r="K2" t="n">
-        <v>0.16666666666666663</v>
+        <v>-0.033333333333333326</v>
       </c>
       <c r="L2" t="n">
         <v>160.0</v>
@@ -2232,10 +2226,10 @@
         <v>132.0</v>
       </c>
       <c r="O2" t="n">
-        <v>120.0</v>
+        <v>125.0</v>
       </c>
       <c r="P2" t="n">
-        <v>40.0</v>
+        <v>41.666666666666664</v>
       </c>
       <c r="Q2" t="n">
         <v>2.9166666666666665</v>
@@ -2253,7 +2247,7 @@
         <v>3.0</v>
       </c>
       <c r="V2" t="n">
-        <v>1.0</v>
+        <v>0.8</v>
       </c>
       <c r="W2" t="n">
         <v>14.0</v>
@@ -2262,10 +2256,10 @@
         <v>0.0</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
@@ -2273,7 +2267,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" t="n">
         <v>40.0</v>
@@ -2282,10 +2276,10 @@
         <v>44.0</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" t="n">
         <v>1.0</v>
@@ -2294,7 +2288,7 @@
         <v>7.0</v>
       </c>
       <c r="I3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J3" t="n">
         <v>0.11111111111111116</v>
@@ -2312,10 +2306,10 @@
         <v>176.0</v>
       </c>
       <c r="O3" t="n">
-        <v>165.0</v>
+        <v>170.0</v>
       </c>
       <c r="P3" t="n">
-        <v>41.25</v>
+        <v>42.5</v>
       </c>
       <c r="Q3" t="n">
         <v>3.888888888888889</v>
@@ -2353,7 +2347,7 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" t="n">
         <v>40.0</v>
@@ -2362,10 +2356,10 @@
         <v>44.0</v>
       </c>
       <c r="E4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
         <v>79</v>
-      </c>
-      <c r="F4" t="s">
-        <v>80</v>
       </c>
       <c r="G4" t="n">
         <v>1.0</v>
@@ -2374,13 +2368,13 @@
         <v>7.0</v>
       </c>
       <c r="I4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.4166666666666665</v>
+        <v>0.08333333333333348</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.2333333333333334</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="L4" t="n">
         <v>160.0</v>
@@ -2392,10 +2386,10 @@
         <v>132.0</v>
       </c>
       <c r="O4" t="n">
-        <v>120.5</v>
+        <v>121.0</v>
       </c>
       <c r="P4" t="n">
-        <v>40.166666666666664</v>
+        <v>40.333333333333336</v>
       </c>
       <c r="Q4" t="n">
         <v>2.9166666666666665</v>
@@ -2404,16 +2398,16 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="S4" t="n">
-        <v>2.5</v>
+        <v>3.0</v>
       </c>
       <c r="T4" t="n">
         <v>3.0</v>
       </c>
       <c r="U4" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="V4" t="n">
-        <v>0.6</v>
+        <v>1.0</v>
       </c>
       <c r="W4" t="n">
         <v>15.0</v>
@@ -2433,7 +2427,7 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" t="n">
         <v>40.0</v>
@@ -2442,10 +2436,10 @@
         <v>44.0</v>
       </c>
       <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
         <v>79</v>
-      </c>
-      <c r="F5" t="s">
-        <v>80</v>
       </c>
       <c r="G5" t="n">
         <v>1.0</v>
@@ -2454,10 +2448,10 @@
         <v>6.0</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J5" t="n">
-        <v>0.08333333333333348</v>
+        <v>-0.4166666666666665</v>
       </c>
       <c r="K5" t="n">
         <v>0.16666666666666663</v>
@@ -2472,10 +2466,10 @@
         <v>132.0</v>
       </c>
       <c r="O5" t="n">
-        <v>120.0</v>
+        <v>120.5</v>
       </c>
       <c r="P5" t="n">
-        <v>40.0</v>
+        <v>40.166666666666664</v>
       </c>
       <c r="Q5" t="n">
         <v>2.9166666666666665</v>
@@ -2484,13 +2478,13 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="S5" t="n">
-        <v>3.0</v>
+        <v>2.5</v>
       </c>
       <c r="T5" t="n">
         <v>3.0</v>
       </c>
       <c r="U5" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="V5" t="n">
         <v>1.0</v>
@@ -2513,7 +2507,7 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" t="n">
         <v>40.0</v>
@@ -2522,10 +2516,10 @@
         <v>44.0</v>
       </c>
       <c r="E6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" t="s">
         <v>79</v>
-      </c>
-      <c r="F6" t="s">
-        <v>80</v>
       </c>
       <c r="G6" t="n">
         <v>1.0</v>
@@ -2534,13 +2528,13 @@
         <v>7.0</v>
       </c>
       <c r="I6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J6" t="n">
         <v>-0.19444444444444464</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.25555555555555554</v>
+        <v>-0.05555555555555558</v>
       </c>
       <c r="L6" t="n">
         <v>160.0</v>
@@ -2552,10 +2546,10 @@
         <v>167.20000000000002</v>
       </c>
       <c r="O6" t="n">
-        <v>157.5</v>
+        <v>152.5</v>
       </c>
       <c r="P6" t="n">
-        <v>41.44736842105263</v>
+        <v>40.13157894736842</v>
       </c>
       <c r="Q6" t="n">
         <v>3.6944444444444446</v>
@@ -2573,7 +2567,7 @@
         <v>3.0</v>
       </c>
       <c r="V6" t="n">
-        <v>0.8</v>
+        <v>1.0</v>
       </c>
       <c r="W6" t="n">
         <v>8.0</v>
@@ -2582,10 +2576,10 @@
         <v>0.0</v>
       </c>
       <c r="Y6" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="Z6" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
@@ -2593,7 +2587,7 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" t="n">
         <v>40.0</v>
@@ -2602,10 +2596,10 @@
         <v>44.0</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7" t="n">
         <v>1.0</v>
@@ -2614,13 +2608,13 @@
         <v>7.0</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J7" t="n">
         <v>0.08333333333333348</v>
       </c>
       <c r="K7" t="n">
-        <v>0.16666666666666663</v>
+        <v>-0.2333333333333334</v>
       </c>
       <c r="L7" t="n">
         <v>160.0</v>
@@ -2653,7 +2647,7 @@
         <v>3.0</v>
       </c>
       <c r="V7" t="n">
-        <v>1.0</v>
+        <v>0.6</v>
       </c>
       <c r="W7" t="n">
         <v>10.0</v>
@@ -2673,7 +2667,7 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" t="n">
         <v>40.0</v>
@@ -2682,10 +2676,10 @@
         <v>44.0</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G8" t="n">
         <v>1.0</v>
@@ -2694,7 +2688,7 @@
         <v>7.0</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J8" t="n">
         <v>0.2777777777777777</v>
@@ -2753,7 +2747,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" t="n">
         <v>40.0</v>
@@ -2762,10 +2756,10 @@
         <v>44.0</v>
       </c>
       <c r="E9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" t="s">
         <v>79</v>
-      </c>
-      <c r="F9" t="s">
-        <v>80</v>
       </c>
       <c r="G9" t="n">
         <v>1.0</v>
@@ -2774,7 +2768,7 @@
         <v>7.0</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J9" t="n">
         <v>-0.38888888888888884</v>
@@ -2792,10 +2786,10 @@
         <v>176.0</v>
       </c>
       <c r="O9" t="n">
-        <v>161.5</v>
+        <v>160.5</v>
       </c>
       <c r="P9" t="n">
-        <v>40.375</v>
+        <v>40.125</v>
       </c>
       <c r="Q9" t="n">
         <v>3.888888888888889</v>
@@ -2833,7 +2827,7 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" t="n">
         <v>40.0</v>
@@ -2842,10 +2836,10 @@
         <v>44.0</v>
       </c>
       <c r="E10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
         <v>79</v>
-      </c>
-      <c r="F10" t="s">
-        <v>80</v>
       </c>
       <c r="G10" t="n">
         <v>1.0</v>
@@ -2854,7 +2848,7 @@
         <v>7.0</v>
       </c>
       <c r="I10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J10" t="n">
         <v>0.36111111111111116</v>
@@ -2924,42 +2918,42 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>82</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>83</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>84</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>85</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>86</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>87</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>88</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>89</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>90</v>
-      </c>
-      <c r="L1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="n">
         <v>0.0</v>
@@ -2977,7 +2971,7 @@
         <v>0.7777777777777777</v>
       </c>
       <c r="G2" t="n">
-        <v>0.47777777777777775</v>
+        <v>0.4555555555555556</v>
       </c>
       <c r="H2" t="n">
         <v>1.0</v>
@@ -2989,10 +2983,10 @@
         <v>9.0</v>
       </c>
       <c r="K2" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="L2" t="n">
-        <v>24.44</v>
+        <v>23.6</v>
       </c>
     </row>
   </sheetData>
@@ -3014,63 +3008,55 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>